<commit_message>
Updated 201 A2 Shelf
x
</commit_message>
<xml_diff>
--- a/donaldson_201_books.xlsx
+++ b/donaldson_201_books.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\colin\Documents\GitHub\student_workers_su21\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kbjur\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406984AF-A921-4416-B310-9AE488FFEA8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A70C203-2418-4911-AE31-BA10F78016D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="310">
   <si>
     <t>Title</t>
   </si>
@@ -856,6 +856,105 @@
   </si>
   <si>
     <t>A3</t>
+  </si>
+  <si>
+    <t>Elementary Partial Differential Equations with Boundary Value Problems</t>
+  </si>
+  <si>
+    <t>Andrews, Larry</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>Higher Mathematics for Engineers and Physics</t>
+  </si>
+  <si>
+    <t>Sokolnikoff, Ivan &amp; Sokolnikoff, Elizabeth</t>
+  </si>
+  <si>
+    <t>Mathematical Methods of Physics</t>
+  </si>
+  <si>
+    <t>Mathews, Jon &amp; Walker, R.L.</t>
+  </si>
+  <si>
+    <t>Magnetism and Very Low Temperatures</t>
+  </si>
+  <si>
+    <t>Casimir, H.B.G.</t>
+  </si>
+  <si>
+    <t>Dictionary of Applied Math for Physics for Engineers and Scientists</t>
+  </si>
+  <si>
+    <t>Previato, Emma</t>
+  </si>
+  <si>
+    <t>A Student's Guide to Vectors and Tensors</t>
+  </si>
+  <si>
+    <t>Advanced Engineering Mathematics</t>
+  </si>
+  <si>
+    <t>Wylie, C.R.</t>
+  </si>
+  <si>
+    <t>Nonlinear Differential Equations</t>
+  </si>
+  <si>
+    <t>Struble, Raimond</t>
+  </si>
+  <si>
+    <t>Theory and Problems of Probability, Random Variable, and Random Processes</t>
+  </si>
+  <si>
+    <t>Hsu, Hwei</t>
+  </si>
+  <si>
+    <t>Theory and Problems of Probability</t>
+  </si>
+  <si>
+    <t>Lipschutz, Seymour &amp; Lipson, Marc</t>
+  </si>
+  <si>
+    <t>Handbook of Physical Calculations</t>
+  </si>
+  <si>
+    <t>Tuma, Jan</t>
+  </si>
+  <si>
+    <t>Advanced Calculus for Applications</t>
+  </si>
+  <si>
+    <t>Hildebrand, Francis</t>
+  </si>
+  <si>
+    <t>Partial Differential Equations in Physics</t>
+  </si>
+  <si>
+    <t>Kreyszig, Erwin</t>
+  </si>
+  <si>
+    <t>Heavisides Operational Calculus</t>
+  </si>
+  <si>
+    <t>Berg, Ernst</t>
+  </si>
+  <si>
+    <t>Div, Grad, Curl, and All That</t>
+  </si>
+  <si>
+    <t>Schey, H.M.</t>
+  </si>
+  <si>
+    <t>Boundary Value Problems</t>
+  </si>
+  <si>
+    <t>Powers, David</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -905,7 +1004,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -925,6 +1024,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -940,7 +1042,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="000"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -948,6 +1049,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="000"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -976,17 +1078,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H1048576" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H1048576" totalsRowShown="0" headerRowDxfId="9" dataDxfId="0">
   <autoFilter ref="A1:H1048576" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Title" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Author" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Year" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="ID #" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{59244217-95DE-4CD7-A971-11EDF8E51C2A}" name="Shelf" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{436E2086-A9D0-42F8-9169-90B74E6B0FC2}" name="Number of" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{5F9613C4-49C8-4E47-BCE1-6AE17FC607A8}" name="Need to manually add to goodreads" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{3745232E-EC3D-4E19-A4D3-3402BBD4120F}" name="Column1" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Title" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Author" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Year" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="ID #" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{59244217-95DE-4CD7-A971-11EDF8E51C2A}" name="Shelf" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{436E2086-A9D0-42F8-9169-90B74E6B0FC2}" name="Number of" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{5F9613C4-49C8-4E47-BCE1-6AE17FC607A8}" name="Need to manually add to goodreads" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{3745232E-EC3D-4E19-A4D3-3402BBD4120F}" name="Column1" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1255,26 +1357,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H186"/>
+  <dimension ref="A1:H163"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="D145" workbookViewId="0">
+      <selection activeCell="H149" sqref="H149"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="33.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="33.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="50.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="33.5703125" style="3"/>
-    <col min="4" max="4" width="33.5703125" style="4"/>
-    <col min="6" max="8" width="33.5703125" style="3"/>
+    <col min="1" max="1" width="50.7265625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="22.7265625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="33.54296875" style="3"/>
+    <col min="4" max="4" width="33.54296875" style="4"/>
+    <col min="5" max="5" width="33.54296875" style="1"/>
+    <col min="6" max="8" width="33.54296875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1296,7 +1399,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -1313,7 +1416,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1330,7 +1433,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -1347,7 +1450,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -1364,7 +1467,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -1381,7 +1484,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -1398,7 +1501,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="29.65" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
@@ -1415,7 +1518,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="29.65" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>19</v>
       </c>
@@ -1432,7 +1535,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
@@ -1449,7 +1552,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
@@ -1466,7 +1569,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
@@ -1483,7 +1586,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
@@ -1500,7 +1603,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
@@ -1517,7 +1620,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>28</v>
       </c>
@@ -1534,7 +1637,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>30</v>
       </c>
@@ -1551,7 +1654,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>31</v>
       </c>
@@ -1568,7 +1671,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>33</v>
       </c>
@@ -1585,7 +1688,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>35</v>
       </c>
@@ -1602,7 +1705,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>37</v>
       </c>
@@ -1619,7 +1722,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>39</v>
       </c>
@@ -1636,7 +1739,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="29.65" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>41</v>
       </c>
@@ -1653,7 +1756,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="29.65" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>43</v>
       </c>
@@ -1673,7 +1776,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="29.65" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>50</v>
       </c>
@@ -1690,7 +1793,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>52</v>
       </c>
@@ -1707,7 +1810,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>54</v>
       </c>
@@ -1724,7 +1827,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>56</v>
       </c>
@@ -1741,7 +1844,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="29.65" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>50</v>
       </c>
@@ -1758,7 +1861,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="29.65" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>58</v>
       </c>
@@ -1775,7 +1878,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="29.65" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>60</v>
       </c>
@@ -1795,7 +1898,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="29.65" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>61</v>
       </c>
@@ -1812,7 +1915,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="29.65" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>63</v>
       </c>
@@ -1832,7 +1935,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="29.65" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>64</v>
       </c>
@@ -1849,7 +1952,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>37</v>
       </c>
@@ -1866,7 +1969,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="29.65" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
         <v>66</v>
       </c>
@@ -1883,7 +1986,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="29.65" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
         <v>67</v>
       </c>
@@ -1900,7 +2003,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>69</v>
       </c>
@@ -1917,7 +2020,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>71</v>
       </c>
@@ -1934,7 +2037,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>74</v>
       </c>
@@ -1951,7 +2054,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>75</v>
       </c>
@@ -1971,7 +2074,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>76</v>
       </c>
@@ -1988,7 +2091,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>77</v>
       </c>
@@ -2005,7 +2108,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>79</v>
       </c>
@@ -2022,7 +2125,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>80</v>
       </c>
@@ -2039,7 +2142,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>82</v>
       </c>
@@ -2056,7 +2159,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>84</v>
       </c>
@@ -2073,7 +2176,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>86</v>
       </c>
@@ -2093,7 +2196,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>87</v>
       </c>
@@ -2110,7 +2213,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>90</v>
       </c>
@@ -2130,7 +2233,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
         <v>84</v>
       </c>
@@ -2150,7 +2253,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>93</v>
       </c>
@@ -2167,7 +2270,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
         <v>94</v>
       </c>
@@ -2184,7 +2287,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="29.65" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
         <v>96</v>
       </c>
@@ -2201,7 +2304,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="29.65" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
         <v>96</v>
       </c>
@@ -2218,7 +2321,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="29.65" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
         <v>98</v>
       </c>
@@ -2235,7 +2338,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
         <v>100</v>
       </c>
@@ -2252,7 +2355,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="29.65" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
         <v>102</v>
       </c>
@@ -2269,7 +2372,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="29.65" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
         <v>104</v>
       </c>
@@ -2286,7 +2389,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
         <v>106</v>
       </c>
@@ -2306,7 +2409,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="29.65" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
         <v>110</v>
       </c>
@@ -2323,7 +2426,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
         <v>109</v>
       </c>
@@ -2340,7 +2443,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
         <v>102</v>
       </c>
@@ -2357,7 +2460,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
         <v>113</v>
       </c>
@@ -2377,7 +2480,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
         <v>115</v>
       </c>
@@ -2394,7 +2497,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
         <v>117</v>
       </c>
@@ -2411,7 +2514,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
         <v>119</v>
       </c>
@@ -2428,7 +2531,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
         <v>121</v>
       </c>
@@ -2445,7 +2548,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="29.65" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
         <v>125</v>
       </c>
@@ -2462,7 +2565,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
         <v>127</v>
       </c>
@@ -2479,7 +2582,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
         <v>129</v>
       </c>
@@ -2496,7 +2599,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
         <v>129</v>
       </c>
@@ -2513,7 +2616,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
         <v>131</v>
       </c>
@@ -2530,7 +2633,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="s">
         <v>133</v>
       </c>
@@ -2547,7 +2650,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="29.65" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A74" s="5" t="s">
         <v>135</v>
       </c>
@@ -2564,7 +2667,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="29.65" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A75" s="5" t="s">
         <v>137</v>
       </c>
@@ -2584,7 +2687,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="s">
         <v>139</v>
       </c>
@@ -2601,7 +2704,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" s="3" t="s">
         <v>141</v>
       </c>
@@ -2618,7 +2721,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
         <v>144</v>
       </c>
@@ -2635,7 +2738,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
         <v>146</v>
       </c>
@@ -2652,7 +2755,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
         <v>148</v>
       </c>
@@ -2669,7 +2772,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="s">
         <v>150</v>
       </c>
@@ -2686,7 +2789,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
         <v>152</v>
       </c>
@@ -2703,7 +2806,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
         <v>154</v>
       </c>
@@ -2723,7 +2826,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="s">
         <v>156</v>
       </c>
@@ -2740,7 +2843,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" s="3" t="s">
         <v>159</v>
       </c>
@@ -2757,7 +2860,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" s="3" t="s">
         <v>161</v>
       </c>
@@ -2774,7 +2877,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" s="3" t="s">
         <v>163</v>
       </c>
@@ -2794,7 +2897,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" s="3" t="s">
         <v>165</v>
       </c>
@@ -2811,7 +2914,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="29.65" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" s="5" t="s">
         <v>167</v>
       </c>
@@ -2828,7 +2931,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
         <v>169</v>
       </c>
@@ -2845,7 +2948,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="s">
         <v>171</v>
       </c>
@@ -2862,7 +2965,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" s="3" t="s">
         <v>173</v>
       </c>
@@ -2879,7 +2982,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="29.65" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A93" s="3" t="s">
         <v>175</v>
       </c>
@@ -2896,7 +2999,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="s">
         <v>177</v>
       </c>
@@ -2913,7 +3016,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95" s="3" t="s">
         <v>179</v>
       </c>
@@ -2933,7 +3036,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96" s="3" t="s">
         <v>181</v>
       </c>
@@ -2950,7 +3053,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="3" t="s">
         <v>183</v>
       </c>
@@ -2967,7 +3070,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="3" t="s">
         <v>185</v>
       </c>
@@ -2984,7 +3087,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="3" t="s">
         <v>187</v>
       </c>
@@ -3001,7 +3104,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
         <v>189</v>
       </c>
@@ -3018,7 +3121,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="3" t="s">
         <v>191</v>
       </c>
@@ -3035,7 +3138,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="3" t="s">
         <v>193</v>
       </c>
@@ -3052,7 +3155,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="3" t="s">
         <v>195</v>
       </c>
@@ -3069,7 +3172,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="3" t="s">
         <v>197</v>
       </c>
@@ -3086,7 +3189,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="29.65" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A105" s="3" t="s">
         <v>199</v>
       </c>
@@ -3103,7 +3206,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="3" t="s">
         <v>201</v>
       </c>
@@ -3120,7 +3223,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="29.65" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A107" s="3" t="s">
         <v>203</v>
       </c>
@@ -3137,7 +3240,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="3" t="s">
         <v>205</v>
       </c>
@@ -3154,7 +3257,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="3" t="s">
         <v>206</v>
       </c>
@@ -3171,7 +3274,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="3" t="s">
         <v>208</v>
       </c>
@@ -3188,7 +3291,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="3" t="s">
         <v>210</v>
       </c>
@@ -3205,7 +3308,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="3" t="s">
         <v>212</v>
       </c>
@@ -3222,7 +3325,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A113" s="3" t="s">
         <v>214</v>
       </c>
@@ -3239,7 +3342,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A114" s="3" t="s">
         <v>216</v>
       </c>
@@ -3259,7 +3362,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="29.65" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A115" s="3" t="s">
         <v>218</v>
       </c>
@@ -3276,7 +3379,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A116" s="3" t="s">
         <v>220</v>
       </c>
@@ -3296,7 +3399,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A117" s="3" t="s">
         <v>222</v>
       </c>
@@ -3316,7 +3419,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A118" s="3" t="s">
         <v>224</v>
       </c>
@@ -3336,7 +3439,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A119" s="3" t="s">
         <v>226</v>
       </c>
@@ -3353,7 +3456,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A120" s="3" t="s">
         <v>228</v>
       </c>
@@ -3370,7 +3473,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A121" s="3" t="s">
         <v>230</v>
       </c>
@@ -3387,7 +3490,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="29.65" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A122" s="3" t="s">
         <v>231</v>
       </c>
@@ -3404,7 +3507,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A123" s="3" t="s">
         <v>234</v>
       </c>
@@ -3421,7 +3524,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A124" s="3" t="s">
         <v>235</v>
       </c>
@@ -3438,7 +3541,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A125" s="3" t="s">
         <v>237</v>
       </c>
@@ -3455,7 +3558,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A126" s="3" t="s">
         <v>239</v>
       </c>
@@ -3472,7 +3575,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A127" s="3" t="s">
         <v>241</v>
       </c>
@@ -3489,7 +3592,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A128" s="3" t="s">
         <v>243</v>
       </c>
@@ -3506,7 +3609,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="29.65" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A129" s="3" t="s">
         <v>245</v>
       </c>
@@ -3523,7 +3626,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A130" s="3" t="s">
         <v>247</v>
       </c>
@@ -3540,7 +3643,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A131" s="3" t="s">
         <v>249</v>
       </c>
@@ -3557,7 +3660,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="29.65" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A132" s="3" t="s">
         <v>251</v>
       </c>
@@ -3574,7 +3677,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A133" s="3" t="s">
         <v>253</v>
       </c>
@@ -3591,7 +3694,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A134" s="3" t="s">
         <v>255</v>
       </c>
@@ -3608,7 +3711,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A135" s="3" t="s">
         <v>257</v>
       </c>
@@ -3625,7 +3728,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="29.65" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A136" s="3" t="s">
         <v>259</v>
       </c>
@@ -3642,7 +3745,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A137" s="3" t="s">
         <v>261</v>
       </c>
@@ -3659,7 +3762,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="29.65" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A138" s="3" t="s">
         <v>263</v>
       </c>
@@ -3676,7 +3779,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A139" s="3" t="s">
         <v>265</v>
       </c>
@@ -3696,7 +3799,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A140" s="3" t="s">
         <v>267</v>
       </c>
@@ -3713,7 +3816,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="141" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A141" s="3" t="s">
         <v>269</v>
       </c>
@@ -3730,7 +3833,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="29.65" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A142" s="3" t="s">
         <v>270</v>
       </c>
@@ -3750,7 +3853,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="143" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A143" s="3" t="s">
         <v>273</v>
       </c>
@@ -3767,7 +3870,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A144" s="3" t="s">
         <v>274</v>
       </c>
@@ -3787,7 +3890,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="1:5" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A145" s="3" t="s">
         <v>237</v>
       </c>
@@ -3804,209 +3907,313 @@
         <v>276</v>
       </c>
     </row>
-    <row r="146" spans="1:5" ht="14.85" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A146" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="C146" s="3">
+        <v>1986</v>
+      </c>
       <c r="D146" s="4">
         <v>145</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" ht="14.85" x14ac:dyDescent="0.25">
+      <c r="E146" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A147" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="B147" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="C147" s="3">
+        <v>1934</v>
+      </c>
       <c r="D147" s="4">
         <v>146</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" ht="14.85" x14ac:dyDescent="0.25">
+      <c r="E147" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A148" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="B148" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="C148" s="3">
+        <v>1964</v>
+      </c>
       <c r="D148" s="4">
         <v>147</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" ht="14.85" x14ac:dyDescent="0.25">
+      <c r="E148" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A149" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="B149" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="C149" s="3">
+        <v>1961</v>
+      </c>
       <c r="D149" s="4">
         <v>148</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" ht="14.85" x14ac:dyDescent="0.25">
+      <c r="E149" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="G149" s="3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A150" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="C150" s="3">
+        <v>2003</v>
+      </c>
       <c r="D150" s="4">
         <v>149</v>
       </c>
-    </row>
-    <row r="151" spans="1:5" ht="14.85" x14ac:dyDescent="0.25">
+      <c r="E150" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A151" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C151" s="3">
+        <v>2012</v>
+      </c>
       <c r="D151" s="4">
         <v>150</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" ht="14.85" x14ac:dyDescent="0.25">
+      <c r="E151" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A152" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="C152" s="3">
+        <v>1960</v>
+      </c>
       <c r="D152" s="4">
         <v>151</v>
       </c>
-    </row>
-    <row r="153" spans="1:5" ht="14.85" x14ac:dyDescent="0.25">
+      <c r="E152" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A153" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="C153" s="3">
+        <v>1962</v>
+      </c>
       <c r="D153" s="4">
         <v>152</v>
       </c>
-    </row>
-    <row r="154" spans="1:5" ht="14.85" x14ac:dyDescent="0.25">
+      <c r="E153" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A154" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C154" s="3">
+        <v>1997</v>
+      </c>
       <c r="D154" s="4">
         <v>153</v>
       </c>
-    </row>
-    <row r="155" spans="1:5" ht="14.85" x14ac:dyDescent="0.25">
+      <c r="E154" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A155" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="B155" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="C155" s="3">
+        <v>2000</v>
+      </c>
       <c r="D155" s="4">
         <v>154</v>
       </c>
-    </row>
-    <row r="156" spans="1:5" ht="14.85" x14ac:dyDescent="0.25">
+      <c r="E155" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A156" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="C156" s="3">
+        <v>1976</v>
+      </c>
       <c r="D156" s="4">
         <v>155</v>
       </c>
-    </row>
-    <row r="157" spans="1:5" ht="14.85" x14ac:dyDescent="0.25">
+      <c r="E156" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A157" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="C157" s="3">
+        <v>1976</v>
+      </c>
       <c r="D157" s="4">
         <v>156</v>
       </c>
-    </row>
-    <row r="158" spans="1:5" ht="14.85" x14ac:dyDescent="0.25">
+      <c r="E157" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A158" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C158" s="3">
+        <v>1949</v>
+      </c>
       <c r="D158" s="4">
         <v>157</v>
       </c>
-    </row>
-    <row r="159" spans="1:5" ht="14.85" x14ac:dyDescent="0.25">
+      <c r="E158" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A159" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="C159" s="3">
+        <v>1972</v>
+      </c>
       <c r="D159" s="4">
         <v>158</v>
       </c>
-    </row>
-    <row r="160" spans="1:5" ht="14.85" x14ac:dyDescent="0.25">
+      <c r="E159" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A160" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="C160" s="3">
+        <v>1936</v>
+      </c>
       <c r="D160" s="4">
         <v>159</v>
       </c>
-    </row>
-    <row r="161" spans="4:4" ht="14.85" x14ac:dyDescent="0.25">
+      <c r="E160" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A161" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C161" s="3">
+        <v>1973</v>
+      </c>
       <c r="D161" s="4">
         <v>160</v>
       </c>
-    </row>
-    <row r="162" spans="4:4" ht="14.85" x14ac:dyDescent="0.25">
+      <c r="E161" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A162" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B162" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C162" s="3">
+        <v>1997</v>
+      </c>
       <c r="D162" s="4">
         <v>161</v>
       </c>
-    </row>
-    <row r="163" spans="4:4" ht="14.85" x14ac:dyDescent="0.25">
+      <c r="E162" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A163" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="B163" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C163" s="3">
+        <v>1979</v>
+      </c>
       <c r="D163" s="4">
         <v>162</v>
       </c>
-    </row>
-    <row r="164" spans="4:4" ht="14.85" x14ac:dyDescent="0.25">
-      <c r="D164" s="4">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="165" spans="4:4" ht="14.85" x14ac:dyDescent="0.25">
-      <c r="D165" s="4">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="166" spans="4:4" ht="14.85" x14ac:dyDescent="0.25">
-      <c r="D166" s="4">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="167" spans="4:4" ht="14.85" x14ac:dyDescent="0.25">
-      <c r="D167" s="4">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="168" spans="4:4" ht="14.85" x14ac:dyDescent="0.25">
-      <c r="D168" s="4">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="169" spans="4:4" ht="14.85" x14ac:dyDescent="0.25">
-      <c r="D169" s="4">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="170" spans="4:4" ht="14.85" x14ac:dyDescent="0.25">
-      <c r="D170" s="4">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="171" spans="4:4" ht="14.85" x14ac:dyDescent="0.25">
-      <c r="D171" s="4">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="172" spans="4:4" ht="14.85" x14ac:dyDescent="0.25">
-      <c r="D172" s="4">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="173" spans="4:4" ht="14.85" x14ac:dyDescent="0.25">
-      <c r="D173" s="4">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="174" spans="4:4" ht="14.85" x14ac:dyDescent="0.25">
-      <c r="D174" s="4">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="175" spans="4:4" ht="14.85" x14ac:dyDescent="0.25">
-      <c r="D175" s="4">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="176" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D176" s="4">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="177" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D177" s="4">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="178" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D178" s="4">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="179" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D179" s="4">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="180" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D180" s="4">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="181" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D181" s="4">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="182" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D182" s="4">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="183" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D183" s="4">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="184" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D184" s="4">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="185" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D185" s="4">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="186" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D186" s="4">
-        <v>185</v>
+      <c r="E163" s="1" t="s">
+        <v>279</v>
       </c>
     </row>
   </sheetData>

</xml_diff>